<commit_message>
Added pokemon info added in S&V DLC (No form diff or evolution)
</commit_message>
<xml_diff>
--- a/Crystal PokeDex/Data/Scarlet&Violet/DLC/特性/特性_简中.xlsx
+++ b/Crystal PokeDex/Data/Scarlet&Violet/DLC/特性/特性_简中.xlsx
@@ -10,7 +10,7 @@
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_1" localSheetId="0">工作表1!$A$1:$G$12</definedName>
+    <definedName name="_1" localSheetId="0">工作表1!$A$1:$G$13</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
   <si>
     <t xml:space="preserve">款待 </t>
   </si>
@@ -152,6 +152,18 @@
   </si>
   <si>
     <t xml:space="preserve">因桃歹郎的招式而陷入中毒状态的对手同时也会陷入混乱状态。 </t>
+  </si>
+  <si>
+    <t>這個特性編號在遊戲中未被使用，參考: https://wiki.52poke.com/wiki/Talk:%E7%89%B9%E6%80%A7%E5%88%97%E8%A1%A8</t>
+  </si>
+  <si>
+    <t>&lt;No Data&gt;</t>
+  </si>
+  <si>
+    <t>？？？</t>
+  </si>
+  <si>
+    <t>&lt;数据暂缺&gt;</t>
   </si>
 </sst>
 </file>
@@ -504,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:G1048576"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -658,75 +670,92 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E10" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12">
+        <v>310</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A13">
         <v>311</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>35</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>36</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>37</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E13" t="s">
         <v>38</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>